<commit_message>
Test interlink for hybrid ac-dc systems
</commit_message>
<xml_diff>
--- a/Debug/UserData_dc.xlsx
+++ b/Debug/UserData_dc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-System-Analysis-Toolbox\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4526B1F8-8130-4890-A0E6-99AA46AA332D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC293480-D027-47AB-B0FD-B249DA7185A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1190,16 +1190,16 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1231,7 +1231,7 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1897,7 +1897,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B0C2B6E-74BD-40FA-8EB6-D64D8C21837A}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>

</xml_diff>